<commit_message>
started processing factor data into modeling data
</commit_message>
<xml_diff>
--- a/data availability_reviewed.xlsx
+++ b/data availability_reviewed.xlsx
@@ -459,14 +459,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="2">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="1">
     <dxf>
       <fill>
         <patternFill>
@@ -773,7 +766,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:W48"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C48" sqref="A1:C48"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -4209,7 +4204,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="D2:W48">
-    <cfRule type="expression" dxfId="1" priority="1">
+    <cfRule type="expression" dxfId="0" priority="1">
       <formula>D2=FALSE</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>